<commit_message>
Update Internet Banking System _SIQ_version1.xlsx
</commit_message>
<xml_diff>
--- a/Requirements/Internet Banking System _SIQ_version1.xlsx
+++ b/Requirements/Internet Banking System _SIQ_version1.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="390" yWindow="525" windowWidth="19815" windowHeight="7365"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="107">
   <si>
     <t>ID</t>
   </si>
@@ -26,9 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve"> bank_sys_Q1</t>
-  </si>
-  <si>
-    <t>what are the interaccount transactions cst can do ?</t>
   </si>
   <si>
     <t>1- check balance.
@@ -42,10 +42,6 @@
     <t>what are the account types cst can have?</t>
   </si>
   <si>
-    <t>1- current acc.
- 2- saving acc.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> bank_sys_Q3</t>
   </si>
   <si>
@@ -85,31 +81,13 @@
     <t>what are the details shall be displayed in each previous transaction?</t>
   </si>
   <si>
-    <t>the amount of money  in green (in case cst recevie) and in red
-( in case cst transfer ) and the ID from which cst received or to 
-which cst transfered.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> bank_sys_Q7</t>
   </si>
   <si>
-    <t>how to display previous transactions filters (dropbox or radio button)?</t>
-  </si>
-  <si>
-    <t>dropbox with three filters (last week , last month , 5 years ago )</t>
-  </si>
-  <si>
     <t xml:space="preserve"> bank_sys_Q8</t>
   </si>
   <si>
     <t>what are the required fields for cst to register an account ?</t>
-  </si>
-  <si>
-    <t>1- username 
- 2-password 
- 3-national ID 
- 4- email
- 5-phone number in which he will receive verification code sms</t>
   </si>
   <si>
     <t xml:space="preserve"> bank_sys_Q9</t>
@@ -138,10 +116,6 @@
   </si>
   <si>
     <t>to what extend must the site be secured?</t>
-  </si>
-  <si>
-    <t>1- (2-way) authentication in registeration. 
- 2- session time out 2mins</t>
   </si>
   <si>
     <t xml:space="preserve"> bank_sys_Q12</t>
@@ -186,22 +160,7 @@
     <t>what are the constrains of the fields in the registration form ?</t>
   </si>
   <si>
-    <t>1- text field with title username accept only characters
- and numbers with max length 32 .
- 2- text field with title password must be strong contains 
-numbers , characters(capital and small) and special
- characters with length from 8 : 12.
- 3- text field with title national ID accepts only numbers
- with length 14 .
- 4- text field with title email 
- 5- text field with title phone number accepts only numbers .
- 6- button with title register at the end of the form .</t>
-  </si>
-  <si>
     <t xml:space="preserve"> bank_sys_Q16</t>
-  </si>
-  <si>
-    <t>what are the constarins of the fields in the login page ?</t>
   </si>
   <si>
     <t>1- text field with title username accept only characters
@@ -227,14 +186,6 @@
     <t xml:space="preserve"> bank_sys_Q18</t>
   </si>
   <si>
-    <t>what is the content of the main page to which cst redirected after
- login or registeration?</t>
-  </si>
-  <si>
-    <t>the mainpage should display all cst accounts (current
- and saving ) in hyperlinks .</t>
-  </si>
-  <si>
     <t xml:space="preserve"> bank_sys_Q19</t>
   </si>
   <si>
@@ -254,14 +205,6 @@
  his account page ?</t>
   </si>
   <si>
-    <t>cst shall be redirected to the transfer page in which 
- 1- two text fields with title amount and account 
-     number .
- 2- dropbox with title bankname (to choose the bank
-     the account number belongs).
- 3- button with title submit .</t>
-  </si>
-  <si>
     <t xml:space="preserve"> bank_sys_Q21</t>
   </si>
   <si>
@@ -269,27 +212,11 @@
 transactions in his account page ?</t>
   </si>
   <si>
-    <t>cst shall be redirected to the prvious transactions
-  page in which there is a dropbox with three filters
- (last week , last month , 5 years ago).
- And button with title view .</t>
-  </si>
-  <si>
     <t xml:space="preserve"> bank_sys_Q22</t>
   </si>
   <si>
     <t>what is the content shall be displayed if the cst click on view in the
  previous transaction page ?</t>
-  </si>
-  <si>
-    <t>1- in case cst has no previous transaction in the 
- determined period : cst shall be redirected to a page 
- in which (no transaction in this period ) textshall be displayed 
- 2- in case cst has previous transaction in the 
- determined period : cst shall be redirected to a page 
- in which he can choose the number of previous transactions
- shall be dispayed in a page from listed items with 3 options
- (10,20,30).</t>
   </si>
   <si>
     <t xml:space="preserve"> bank_sys_Q23</t>
@@ -311,17 +238,9 @@
     <t>what are the nonfunctional requirements?</t>
   </si>
   <si>
-    <t>1- load : 2000 TPS
- 2- performance : the avg latenency of 90% percent is 7 sec 
-by maximum for each response on a request hits the backend .</t>
-  </si>
-  <si>
     <t xml:space="preserve"> bank_sys_Q25</t>
   </si>
   <si>
-    <t>what is the accepted minimum number of characters in the username textfield?</t>
-  </si>
-  <si>
     <t>one character .</t>
   </si>
   <si>
@@ -337,16 +256,10 @@
     <t xml:space="preserve"> bank_sys_Q27</t>
   </si>
   <si>
-    <t xml:space="preserve">what is the max length in the phone number textfield ? </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 20 numbers </t>
   </si>
   <si>
     <t xml:space="preserve"> bank_sys_Q28</t>
-  </si>
-  <si>
-    <t>what is the default value of the dropbox in the page of previous transactions ?</t>
   </si>
   <si>
     <t>default value can be last week .</t>
@@ -380,76 +293,183 @@
     <t xml:space="preserve"> bank_sys_Q31</t>
   </si>
   <si>
-    <t>what is the content shall be displayed to the admin after login or registeration ?</t>
+    <t xml:space="preserve"> bank_sys_Q32</t>
+  </si>
+  <si>
+    <t>what is the content shall be displayed to the admin if he clicks on add new 
+account hyperlink  ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bank_sys_Q33</t>
+  </si>
+  <si>
+    <t>what are the constrains of the staff ID test field ?</t>
+  </si>
+  <si>
+    <t>shall accept only numbers by max 6.</t>
+  </si>
+  <si>
+    <t>what are the inter account transactions cst can do ?</t>
+  </si>
+  <si>
+    <t>1- current account
+ 2- saving account</t>
+  </si>
+  <si>
+    <t>1- username 
+ 2-password 
+ 3-national ID 
+ 4- email
+ 5-phone number ( which cst will receive verification code sms)</t>
+  </si>
+  <si>
+    <t>1- text field with title username accept only characters
+ and numbers with max length 32 .
+ 2- text field with title password must be strong contains 
+numbers , characters(capital and small) and special
+ characters with length from 8 : 12.
+ 3- text field with title national ID accepts only numbers
+ with length 14 .
+ 4- text field with title email with right email format
+ 5- text field with title phone number accepts only numbers .
+ 6- button with title register at the end of the form .</t>
+  </si>
+  <si>
+    <t>performance testing only required from all types of nonfunctional 
+1- load : 2000 TPS
+ 2- performance : the avg latency of 90% percent is 7 sec 
+by maximum for each response on a request hits the backend .</t>
+  </si>
+  <si>
+    <t>what are the required fields for admin to login to his account ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bank_sys_Q34</t>
+  </si>
+  <si>
+    <t>what is the out of scope of this project?</t>
+  </si>
+  <si>
+    <t>all nonfunctional types of testing except load performance</t>
+  </si>
+  <si>
+    <t>the amount of money  in green (in case cst receive) and in red
+( in case cst transfer ) and the ID from which cst received or to 
+which cst transferred.</t>
+  </si>
+  <si>
+    <t>how to display previous transactions filters (drop box or radio button)?</t>
+  </si>
+  <si>
+    <t>drop box with three filters (last week , last month , 5 years ago )</t>
+  </si>
+  <si>
+    <t>1- (2-way) authentication in registration. 
+ 2- session time out 2mins</t>
+  </si>
+  <si>
+    <t>what are the constrains of the fields in the login page ?</t>
+  </si>
+  <si>
+    <t>what is the content of the main page to which cst redirected after
+ login or registration?</t>
+  </si>
+  <si>
+    <t>the main page should display all cst accounts (current
+ and saving ) in hyperlinks .</t>
+  </si>
+  <si>
+    <t>cst shall be redirected to the transfer page in which 
+ 1- two text fields with title amount and account 
+     number .
+ 2- drop box with title banks names (to choose the bank
+     the account number (which will cst transfer money to)  belongs).
+ 3- button with title submit .</t>
+  </si>
+  <si>
+    <t>cst shall be redirected to the previous transactions
+  page in which there is a drop box with three filters
+ (last week , last month , 5 years ago).
+ And button with title view .</t>
+  </si>
+  <si>
+    <t>1- in case cst has no previous transaction in the 
+ determined period : cst shall be redirected to a page 
+ in which (no transaction in this period ) text shall be displayed 
+ 2- in case cst has previous transaction in the 
+ determined period : cst shall be redirected to a page 
+ in which he can choose the number of previous transactions
+ shall be displayed in a page from listed items with 3 options
+ (10,20,30).</t>
+  </si>
+  <si>
+    <t>what is the accepted minimum number of characters in the username text field?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what is the max length in the phone number text field ? </t>
+  </si>
+  <si>
+    <t>what is the default value of the drop box in the page of previous transactions ?</t>
+  </si>
+  <si>
+    <t>what is the content shall be displayed to the admin after login or registration ?</t>
   </si>
   <si>
     <t xml:space="preserve">admin shall be redirected to a page with 
 1- text field with title id  (to enter cst id )
 2- 2 buttons : first button with title delete to delete cst ID .
     second button with title view to redirect to cst account page .
-3- huper link : add new account . </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> bank_sys_Q32</t>
-  </si>
-  <si>
-    <t>what is the content shall be displayed to the admin if he clicks on add new 
-account hyperlink  ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin shall be redirected to the normal registeration page in which 
+3- hyper link : add new account . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin shall be redirected to the normal registration page in which 
 he can enter all cst data and no need to send a verification code to the 
 phone number in this case. 
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> bank_sys_Q33</t>
-  </si>
-  <si>
-    <t>what are the constrains of the staff ID test field ?</t>
-  </si>
-  <si>
-    <t>shall accept only numbers by max 6.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="6">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -459,7 +479,13 @@
     </fill>
   </fills>
   <borders count="3">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FFCCCCCC"/>
@@ -473,98 +499,369 @@
       <bottom style="thin">
         <color rgb="FFCCCCCC"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="27.86"/>
-    <col customWidth="1" min="2" max="2" width="65.57"/>
-    <col customWidth="1" min="3" max="3" width="59.57"/>
-    <col customWidth="1" min="4" max="4" width="60.43"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="65.5703125" customWidth="1"/>
+    <col min="3" max="3" width="59.5703125" customWidth="1"/>
+    <col min="4" max="4" width="60.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,16 +897,16 @@
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" ht="43.5">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="18" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7" t="s">
-        <v>6</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -634,16 +931,16 @@
       <c r="Y2" s="8"/>
       <c r="Z2" s="8"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:26" ht="30">
       <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="9" t="s">
-        <v>9</v>
+      <c r="D3" s="19" t="s">
+        <v>83</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -668,16 +965,16 @@
       <c r="Y3" s="8"/>
       <c r="Z3" s="8"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:26">
       <c r="A4" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -702,18 +999,18 @@
       <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:26">
       <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="D5" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
@@ -738,16 +1035,16 @@
       <c r="Y5" s="8"/>
       <c r="Z5" s="8"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:26" ht="43.5">
       <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="18" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="7" t="s">
-        <v>19</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -772,16 +1069,16 @@
       <c r="Y6" s="8"/>
       <c r="Z6" s="8"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:26" ht="57.75">
       <c r="A7" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="8"/>
-      <c r="D7" s="7" t="s">
-        <v>22</v>
+      <c r="D7" s="18" t="s">
+        <v>91</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -806,16 +1103,16 @@
       <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:26">
       <c r="A8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="7" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -840,18 +1137,18 @@
       <c r="Y8" s="8"/>
       <c r="Z8" s="8"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:26" ht="86.25">
       <c r="A9" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>84</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -876,18 +1173,18 @@
       <c r="Y9" s="8"/>
       <c r="Z9" s="8"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:26">
       <c r="A10" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
@@ -912,16 +1209,16 @@
       <c r="Y10" s="8"/>
       <c r="Z10" s="8"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:26" ht="45">
       <c r="A11" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="9" t="s">
-        <v>34</v>
+      <c r="D11" s="19" t="s">
+        <v>28</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -946,16 +1243,16 @@
       <c r="Y11" s="8"/>
       <c r="Z11" s="8"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:26" ht="29.25">
       <c r="A12" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C12" s="8"/>
-      <c r="D12" s="7" t="s">
-        <v>37</v>
+      <c r="D12" s="18" t="s">
+        <v>94</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -980,16 +1277,16 @@
       <c r="Y12" s="8"/>
       <c r="Z12" s="8"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:26" ht="57.75">
       <c r="A13" s="6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C13" s="12"/>
-      <c r="D13" s="11" t="s">
-        <v>40</v>
+      <c r="D13" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
@@ -1014,18 +1311,18 @@
       <c r="Y13" s="12"/>
       <c r="Z13" s="12"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:26">
       <c r="A14" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1050,16 +1347,16 @@
       <c r="Y14" s="8"/>
       <c r="Z14" s="8"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:26" ht="57.75">
       <c r="A15" s="6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="7" t="s">
-        <v>46</v>
+      <c r="D15" s="18" t="s">
+        <v>39</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1084,16 +1381,16 @@
       <c r="Y15" s="8"/>
       <c r="Z15" s="8"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:26" ht="143.25">
       <c r="A16" s="6" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C16" s="8"/>
-      <c r="D16" s="7" t="s">
-        <v>49</v>
+      <c r="D16" s="18" t="s">
+        <v>85</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1118,16 +1415,16 @@
       <c r="Y16" s="8"/>
       <c r="Z16" s="8"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:26" ht="100.5">
       <c r="A17" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>51</v>
+        <v>42</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>95</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="7" t="s">
-        <v>52</v>
+      <c r="D17" s="18" t="s">
+        <v>43</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1152,16 +1449,16 @@
       <c r="Y17" s="8"/>
       <c r="Z17" s="8"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:26" ht="45">
       <c r="A18" s="6" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C18" s="8"/>
-      <c r="D18" s="9" t="s">
-        <v>55</v>
+      <c r="D18" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1186,16 +1483,16 @@
       <c r="Y18" s="8"/>
       <c r="Z18" s="8"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:26" ht="30">
       <c r="A19" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>57</v>
+        <v>47</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>96</v>
       </c>
       <c r="C19" s="8"/>
-      <c r="D19" s="9" t="s">
-        <v>58</v>
+      <c r="D19" s="19" t="s">
+        <v>97</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1220,16 +1517,16 @@
       <c r="Y19" s="8"/>
       <c r="Z19" s="8"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:26" ht="45">
       <c r="A20" s="6" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C20" s="8"/>
-      <c r="D20" s="9" t="s">
-        <v>61</v>
+      <c r="D20" s="19" t="s">
+        <v>50</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1254,16 +1551,16 @@
       <c r="Y20" s="8"/>
       <c r="Z20" s="8"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:26" ht="100.5">
       <c r="A21" s="6" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="7" t="s">
-        <v>64</v>
+      <c r="D21" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -1288,16 +1585,16 @@
       <c r="Y21" s="8"/>
       <c r="Z21" s="8"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:26" ht="57.75">
       <c r="A22" s="6" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C22" s="8"/>
-      <c r="D22" s="7" t="s">
-        <v>67</v>
+      <c r="D22" s="18" t="s">
+        <v>99</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -1322,16 +1619,16 @@
       <c r="Y22" s="8"/>
       <c r="Z22" s="8"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:26" ht="114.75">
       <c r="A23" s="6" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="7" t="s">
-        <v>70</v>
+      <c r="D23" s="18" t="s">
+        <v>100</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
@@ -1356,15 +1653,15 @@
       <c r="Y23" s="8"/>
       <c r="Z23" s="8"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:26" ht="86.25">
       <c r="A24" s="13" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>73</v>
+        <v>58</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>59</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
@@ -1390,16 +1687,16 @@
       <c r="Y24" s="15"/>
       <c r="Z24" s="15"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:26" ht="86.25">
       <c r="A25" s="6" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="7" t="s">
-        <v>76</v>
+      <c r="D25" s="18" t="s">
+        <v>86</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
@@ -1424,15 +1721,15 @@
       <c r="Y25" s="8"/>
       <c r="Z25" s="8"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="13" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
@@ -1458,15 +1755,15 @@
       <c r="Y26" s="17"/>
       <c r="Z26" s="17"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:26" ht="15.75" customHeight="1">
       <c r="A27" s="13" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
@@ -1492,15 +1789,15 @@
       <c r="Y27" s="17"/>
       <c r="Z27" s="17"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:26" ht="15.75" customHeight="1">
       <c r="A28" s="13" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
@@ -1526,15 +1823,15 @@
       <c r="Y28" s="17"/>
       <c r="Z28" s="17"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:26" ht="15.75" customHeight="1">
       <c r="A29" s="13" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
@@ -1560,15 +1857,15 @@
       <c r="Y29" s="17"/>
       <c r="Z29" s="17"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:26" ht="15.75" customHeight="1">
       <c r="A30" s="13" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>91</v>
+        <v>72</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>73</v>
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
@@ -1594,15 +1891,15 @@
       <c r="Y30" s="17"/>
       <c r="Z30" s="17"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:26" ht="15.75" customHeight="1">
       <c r="A31" s="13" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="D31" s="17"/>
       <c r="E31" s="17"/>
@@ -1628,15 +1925,15 @@
       <c r="Y31" s="17"/>
       <c r="Z31" s="17"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:26" ht="15.75" customHeight="1">
       <c r="A32" s="13" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>96</v>
+        <v>104</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>105</v>
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="17"/>
@@ -1662,15 +1959,15 @@
       <c r="Y32" s="17"/>
       <c r="Z32" s="17"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:26" ht="15.75" customHeight="1">
       <c r="A33" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>99</v>
+        <v>77</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>106</v>
       </c>
       <c r="D33" s="17"/>
       <c r="E33" s="17"/>
@@ -1696,15 +1993,15 @@
       <c r="Y33" s="17"/>
       <c r="Z33" s="17"/>
     </row>
-    <row r="34">
-      <c r="A34" s="13" t="s">
-        <v>100</v>
+    <row r="34" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A34" s="14" t="s">
+        <v>79</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="D34" s="17"/>
       <c r="E34" s="17"/>
@@ -1730,7 +2027,18 @@
       <c r="Y34" s="17"/>
       <c r="Z34" s="17"/>
     </row>
+    <row r="35" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A35" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>